<commit_message>
work 1.2.1 week report with excel
</commit_message>
<xml_diff>
--- a/files_samples/Итоги 04.11-10.11.2024.xlsx
+++ b/files_samples/Итоги 04.11-10.11.2024.xlsx
@@ -1305,7 +1305,7 @@
         <v>4.758620689655173</v>
       </c>
       <c r="D4" s="16" t="n">
-        <v>4.892857142857143</v>
+        <v>5</v>
       </c>
       <c r="E4" s="9" t="n">
         <v>1</v>
@@ -1513,7 +1513,7 @@
         <v>4.876923076923077</v>
       </c>
       <c r="D13" s="16" t="n">
-        <v>4.9375</v>
+        <v>5</v>
       </c>
       <c r="E13" s="9" t="n">
         <v>2</v>
@@ -1536,7 +1536,7 @@
         <v>4.726141078838174</v>
       </c>
       <c r="D14" s="16" t="n">
-        <v>4.824786324786325</v>
+        <v>4.857758620689655</v>
       </c>
       <c r="E14" s="9" t="n">
         <v>62</v>
@@ -2158,7 +2158,7 @@
         <v>4.551401869158878</v>
       </c>
       <c r="D41" s="16" t="n">
-        <v>4.551401869158878</v>
+        <v>4.584905660377358</v>
       </c>
       <c r="E41" s="9" t="n">
         <v>31</v>
@@ -2296,7 +2296,7 @@
         <v>4.75</v>
       </c>
       <c r="D47" s="16" t="n">
-        <v>4.75</v>
+        <v>4.869565217391305</v>
       </c>
       <c r="E47" s="9" t="n">
         <v>0</v>
@@ -2399,10 +2399,20 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="9" t="n"/>
-      <c r="B52" s="15" t="n"/>
-      <c r="C52" s="16" t="n"/>
-      <c r="D52" s="16" t="n"/>
+      <c r="A52" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Павликов Илья Сергеевич </t>
+        </is>
+      </c>
+      <c r="B52" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C52" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" s="16" t="n">
+        <v>1</v>
+      </c>
       <c r="E52" s="9" t="n">
         <v>0</v>
       </c>
@@ -2412,10 +2422,20 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="9" t="n"/>
-      <c r="B53" s="15" t="n"/>
-      <c r="C53" s="16" t="n"/>
-      <c r="D53" s="16" t="n"/>
+      <c r="A53" s="9" t="inlineStr">
+        <is>
+          <t>Верле Каролина Валерьевна (Обучение 2)</t>
+        </is>
+      </c>
+      <c r="B53" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C53" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D53" s="16" t="n">
+        <v>1</v>
+      </c>
       <c r="E53" s="9" t="n">
         <v>0</v>
       </c>
@@ -2425,10 +2445,20 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="9" t="n"/>
-      <c r="B54" s="15" t="n"/>
-      <c r="C54" s="16" t="n"/>
-      <c r="D54" s="16" t="n"/>
+      <c r="A54" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Довыдович Алиса Станиславовна </t>
+        </is>
+      </c>
+      <c r="B54" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C54" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" s="16" t="n">
+        <v>1</v>
+      </c>
       <c r="E54" s="9" t="n">
         <v>0</v>
       </c>
@@ -2438,10 +2468,20 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="9" t="n"/>
-      <c r="B55" s="15" t="n"/>
-      <c r="C55" s="16" t="n"/>
-      <c r="D55" s="16" t="n"/>
+      <c r="A55" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Шептунова Софья Денисовна</t>
+        </is>
+      </c>
+      <c r="B55" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C55" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" s="16" t="n">
+        <v>1</v>
+      </c>
       <c r="E55" s="9" t="n">
         <v>0</v>
       </c>

</xml_diff>